<commit_message>
Changes made to ConnectingWeather, gmailReader, and some new files for testing
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/2018 Data/DailyReports/ToRemoveFile.xlsx
+++ b/Excel & CSV Sheets/2018 Data/DailyReports/ToRemoveFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="61">
   <si>
     <t>Index</t>
   </si>
@@ -61,118 +61,142 @@
     <t>Humidity</t>
   </si>
   <si>
+    <t>Month</t>
+  </si>
+  <si>
     <t>Visibility</t>
   </si>
   <si>
-    <t>2018-07-16</t>
-  </si>
-  <si>
-    <t>11:03:16</t>
-  </si>
-  <si>
-    <t>11:02:44</t>
-  </si>
-  <si>
-    <t>10:42:00</t>
-  </si>
-  <si>
-    <t>09:59:31</t>
-  </si>
-  <si>
-    <t>09:57:29</t>
-  </si>
-  <si>
-    <t>09:57:13</t>
-  </si>
-  <si>
-    <t>05:24:00</t>
-  </si>
-  <si>
-    <t>03:54:48</t>
-  </si>
-  <si>
-    <t>03:54:01</t>
-  </si>
-  <si>
-    <t>03:05:35</t>
-  </si>
-  <si>
-    <t>01:07:52</t>
-  </si>
-  <si>
-    <t>01:06:39</t>
-  </si>
-  <si>
-    <t>01:06:29</t>
-  </si>
-  <si>
-    <t>01:06:10</t>
-  </si>
-  <si>
-    <t>09:06:50</t>
+    <t>2018-07-15</t>
+  </si>
+  <si>
+    <t>07:55:11</t>
+  </si>
+  <si>
+    <t>07:55:04</t>
+  </si>
+  <si>
+    <t>07:54:42</t>
+  </si>
+  <si>
+    <t>06:44:45</t>
+  </si>
+  <si>
+    <t>04:54:34</t>
+  </si>
+  <si>
+    <t>03:35:38</t>
+  </si>
+  <si>
+    <t>03:26:02</t>
+  </si>
+  <si>
+    <t>03:25:41</t>
+  </si>
+  <si>
+    <t>03:25:31</t>
+  </si>
+  <si>
+    <t>02:33:07</t>
+  </si>
+  <si>
+    <t>02:30:56</t>
+  </si>
+  <si>
+    <t>02:25:52</t>
+  </si>
+  <si>
+    <t>02:25:18</t>
+  </si>
+  <si>
+    <t>03:00:55</t>
+  </si>
+  <si>
+    <t>02:59:32</t>
+  </si>
+  <si>
+    <t>02:47:28</t>
+  </si>
+  <si>
+    <t>02:37:54</t>
+  </si>
+  <si>
+    <t>02:23:21</t>
+  </si>
+  <si>
+    <t>No Injuries</t>
   </si>
   <si>
     <t>Injuries</t>
   </si>
   <si>
-    <t>No Injuries</t>
-  </si>
-  <si>
     <t>Unknown Injuries</t>
   </si>
   <si>
-    <t>15617 May Rd</t>
-  </si>
-  <si>
-    <t>1514-1599 Prater Rd</t>
-  </si>
-  <si>
-    <t>18250 - 18289 Interstate 24 Wb</t>
-  </si>
-  <si>
-    <t>18250-18299 Interstate 24  East Bound</t>
-  </si>
-  <si>
-    <t>1440 INTERSTATE 75  NORTH BOUND</t>
-  </si>
-  <si>
-    <t>1101 Dayton Blvd</t>
-  </si>
-  <si>
-    <t>Gunbarrel Rd / E Brainerd Rd</t>
-  </si>
-  <si>
-    <t>6730 - 6999 Shirley Pond Rd</t>
-  </si>
-  <si>
-    <t>100 - 199 Riverside Dr</t>
+    <t>Entrapment</t>
+  </si>
+  <si>
+    <t>400 Interstate 75 Nb</t>
+  </si>
+  <si>
+    <t>400 INTERSTATE 75 NB</t>
+  </si>
+  <si>
+    <t>740 MONTLAKE RD</t>
+  </si>
+  <si>
+    <t>Bonny Oaks Dr / Jersey Pike</t>
+  </si>
+  <si>
+    <t>321 Browns Ferry Rd</t>
+  </si>
+  <si>
+    <t>3746 - 3799 Cummings Hwy</t>
+  </si>
+  <si>
+    <t>1800 GREENWOOD RD</t>
+  </si>
+  <si>
+    <t>3131 Mountain Creek Rd</t>
+  </si>
+  <si>
+    <t>1013 S Greenwood Ave</t>
+  </si>
+  <si>
+    <t>1400 Cowart St</t>
+  </si>
+  <si>
+    <t>18500 Interstate 24 Eb</t>
+  </si>
+  <si>
+    <t>18520 INTERSTATE 24 EB</t>
+  </si>
+  <si>
+    <t>7200 LEE HWY</t>
+  </si>
+  <si>
+    <t>CHATTANOOGA</t>
   </si>
   <si>
     <t>HAMILTON COUNTY</t>
   </si>
   <si>
-    <t>EAST RIDGE</t>
-  </si>
-  <si>
-    <t>RED BANK</t>
-  </si>
-  <si>
-    <t>CHATTANOOGA</t>
-  </si>
-  <si>
     <t>partly-cloudy-day</t>
   </si>
   <si>
     <t>partly-cloudy-night</t>
   </si>
   <si>
-    <t>Humid and Mostly Cloudy</t>
-  </si>
-  <si>
-    <t>Humid and Partly Cloudy</t>
+    <t>clear-night</t>
+  </si>
+  <si>
+    <t>Mostly Cloudy</t>
   </si>
   <si>
     <t>Partly Cloudy</t>
+  </si>
+  <si>
+    <t>Clear</t>
   </si>
 </sst>
 </file>
@@ -530,13 +554,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,58 +609,64 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>35374910</v>
+        <v>35024320</v>
       </c>
       <c r="E2">
-        <v>85064244</v>
+        <v>85174239</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="M2">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N2">
-        <v>80.31999999999999</v>
+        <v>72.56999999999999</v>
       </c>
       <c r="O2">
-        <v>75.04000000000001</v>
+        <v>70.98999999999999</v>
       </c>
       <c r="P2">
-        <v>0.84</v>
+        <v>0.95</v>
       </c>
       <c r="Q2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R2">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -644,49 +674,52 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>35374910</v>
+        <v>35024320</v>
       </c>
       <c r="E3">
-        <v>85064244</v>
+        <v>85174239</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="M3">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="N3">
-        <v>80.31999999999999</v>
+        <v>72.56999999999999</v>
       </c>
       <c r="O3">
-        <v>75.04000000000001</v>
+        <v>70.98999999999999</v>
       </c>
       <c r="P3">
-        <v>0.84</v>
+        <v>0.95</v>
       </c>
       <c r="Q3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R3">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -694,646 +727,950 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <v>34988219</v>
+        <v>35024320</v>
       </c>
       <c r="E4">
-        <v>85216439</v>
+        <v>85174239</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="M4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N4">
-        <v>78.18000000000001</v>
+        <v>72.56999999999999</v>
       </c>
       <c r="O4">
-        <v>72.7</v>
+        <v>70.98999999999999</v>
       </c>
       <c r="P4">
-        <v>0.83</v>
+        <v>0.95</v>
       </c>
       <c r="Q4">
-        <v>5.45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R4">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>35020588</v>
+        <v>35024320</v>
       </c>
       <c r="E5">
-        <v>85259991</v>
+        <v>85174239</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="M5">
+        <v>7</v>
+      </c>
+      <c r="N5">
+        <v>72.56999999999999</v>
+      </c>
+      <c r="O5">
+        <v>70.98999999999999</v>
+      </c>
+      <c r="P5">
+        <v>0.95</v>
+      </c>
+      <c r="Q5">
+        <v>7</v>
+      </c>
+      <c r="R5">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="1">
         <v>9</v>
       </c>
-      <c r="N5">
-        <v>75.76000000000001</v>
-      </c>
-      <c r="O5">
-        <v>72.48</v>
-      </c>
-      <c r="P5">
-        <v>0.9</v>
-      </c>
-      <c r="Q5">
-        <v>5.23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="1">
-        <v>17</v>
-      </c>
       <c r="B6">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>35016792</v>
+        <v>35237122</v>
       </c>
       <c r="E6">
-        <v>85255420</v>
+        <v>85223951</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="L6" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N6">
-        <v>75.87</v>
+        <v>70.75</v>
       </c>
       <c r="O6">
-        <v>72.45999999999999</v>
+        <v>70.66</v>
       </c>
       <c r="P6">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>5.28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R6">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7">
-        <v>35016792</v>
+        <v>35073644</v>
       </c>
       <c r="E7">
-        <v>85255420</v>
+        <v>85190340</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="J7" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="L7" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="M7">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N7">
-        <v>75.87</v>
+        <v>73.63</v>
       </c>
       <c r="O7">
-        <v>72.45999999999999</v>
+        <v>71.31</v>
       </c>
       <c r="P7">
-        <v>0.89</v>
+        <v>0.92</v>
       </c>
       <c r="Q7">
-        <v>5.28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R7">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="1">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B8">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D8">
-        <v>35120082</v>
+        <v>35030883</v>
       </c>
       <c r="E8">
-        <v>85043852</v>
+        <v>85363767</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K8" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L8" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="M8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N8">
-        <v>73.63</v>
+        <v>73.91</v>
       </c>
       <c r="O8">
-        <v>72.09</v>
+        <v>71.65000000000001</v>
       </c>
       <c r="P8">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="Q8">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="1">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B9">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D9">
-        <v>35075367</v>
+        <v>35018464</v>
       </c>
       <c r="E9">
-        <v>85319310</v>
+        <v>85382482</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="K9" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L9" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="M9">
         <v>3</v>
       </c>
       <c r="N9">
-        <v>73.72</v>
+        <v>73.66</v>
       </c>
       <c r="O9">
-        <v>71.92</v>
+        <v>71.66</v>
       </c>
       <c r="P9">
-        <v>0.9399999999999999</v>
+        <v>0.93</v>
       </c>
       <c r="Q9">
-        <v>5.86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R9">
+        <v>4.73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="1">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B10">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D10">
-        <v>35075367</v>
+        <v>35056302</v>
       </c>
       <c r="E10">
-        <v>85319310</v>
+        <v>85241207</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="K10" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="M10">
         <v>3</v>
       </c>
       <c r="N10">
-        <v>73.72</v>
+        <v>73.38</v>
       </c>
       <c r="O10">
-        <v>71.92</v>
+        <v>71.79000000000001</v>
       </c>
       <c r="P10">
-        <v>0.9399999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="Q10">
-        <v>5.86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R10">
+        <v>6.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="1">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B11">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D11">
-        <v>35015214</v>
+        <v>35056302</v>
       </c>
       <c r="E11">
-        <v>85163699</v>
+        <v>85241207</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
         <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="K11" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L11" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="M11">
         <v>3</v>
       </c>
       <c r="N11">
-        <v>74.25</v>
+        <v>73.38</v>
       </c>
       <c r="O11">
-        <v>71.93000000000001</v>
+        <v>71.79000000000001</v>
       </c>
       <c r="P11">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
       <c r="Q11">
-        <v>6.77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R11">
+        <v>6.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="1">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B12">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D12">
-        <v>35173566</v>
+        <v>35120041</v>
       </c>
       <c r="E12">
-        <v>85088409</v>
+        <v>85315464</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
         <v>27</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="J12" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K12" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="L12" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12">
-        <v>74.04000000000001</v>
+        <v>74.98</v>
       </c>
       <c r="O12">
-        <v>72.78</v>
+        <v>71.89</v>
       </c>
       <c r="P12">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="Q12">
-        <v>7.76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R12">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="1">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B13">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D13">
-        <v>35173566</v>
+        <v>35120041</v>
       </c>
       <c r="E13">
-        <v>85088409</v>
+        <v>85315464</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s">
         <v>28</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="J13" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K13" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="L13" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N13">
-        <v>74.04000000000001</v>
+        <v>74.98</v>
       </c>
       <c r="O13">
-        <v>72.78</v>
+        <v>71.89</v>
       </c>
       <c r="P13">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="Q13">
-        <v>7.76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R13">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="1">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B14">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D14">
-        <v>35170745</v>
+        <v>35031909</v>
       </c>
       <c r="E14">
-        <v>85085493</v>
+        <v>85285044</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
         <v>29</v>
       </c>
       <c r="H14" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J14" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K14" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L14" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14">
-        <v>74.19</v>
+        <v>75.23</v>
       </c>
       <c r="O14">
-        <v>72.81999999999999</v>
+        <v>71.84999999999999</v>
       </c>
       <c r="P14">
-        <v>0.96</v>
+        <v>0.89</v>
       </c>
       <c r="Q14">
-        <v>7.92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R14">
+        <v>6.01</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="1">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B15">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D15">
-        <v>35170745</v>
+        <v>35031909</v>
       </c>
       <c r="E15">
-        <v>85085493</v>
+        <v>85285044</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
         <v>30</v>
       </c>
       <c r="H15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I15" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="K15" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L15" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15">
-        <v>74.19</v>
+        <v>75.23</v>
       </c>
       <c r="O15">
-        <v>72.81999999999999</v>
+        <v>71.84999999999999</v>
       </c>
       <c r="P15">
-        <v>0.96</v>
+        <v>0.89</v>
       </c>
       <c r="Q15">
-        <v>7.92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+        <v>7</v>
+      </c>
+      <c r="R15">
+        <v>6.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="1">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B16">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D16">
-        <v>35056620</v>
+        <v>35038239</v>
       </c>
       <c r="E16">
-        <v>85309646</v>
+        <v>85309338</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G16" t="s">
         <v>31</v>
       </c>
       <c r="H16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>73.84999999999999</v>
+      </c>
+      <c r="O16">
+        <v>71.62</v>
+      </c>
+      <c r="P16">
+        <v>0.93</v>
+      </c>
+      <c r="Q16">
+        <v>7</v>
+      </c>
+      <c r="R16">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="1">
+        <v>74</v>
+      </c>
+      <c r="B17">
+        <v>74</v>
+      </c>
+      <c r="D17">
+        <v>35038239</v>
+      </c>
+      <c r="E17">
+        <v>85309338</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
         <v>32</v>
       </c>
-      <c r="I16" t="s">
-        <v>43</v>
-      </c>
-      <c r="J16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" t="s">
-        <v>48</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="H17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" t="s">
+        <v>57</v>
+      </c>
+      <c r="L17" t="s">
+        <v>60</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>75.36</v>
+      </c>
+      <c r="O17">
+        <v>71.72</v>
+      </c>
+      <c r="P17">
+        <v>0.89</v>
+      </c>
+      <c r="Q17">
+        <v>7</v>
+      </c>
+      <c r="R17">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="1">
+        <v>76</v>
+      </c>
+      <c r="B18">
+        <v>76</v>
+      </c>
+      <c r="D18">
+        <v>35004334</v>
+      </c>
+      <c r="E18">
+        <v>85221655</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" t="s">
         <v>50</v>
       </c>
-      <c r="M16">
-        <v>9</v>
-      </c>
-      <c r="N16">
-        <v>76.37</v>
-      </c>
-      <c r="O16">
-        <v>72.40000000000001</v>
-      </c>
-      <c r="P16">
-        <v>0.88</v>
-      </c>
-      <c r="Q16">
-        <v>4.92</v>
+      <c r="J18" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>74.88</v>
+      </c>
+      <c r="O18">
+        <v>71.87</v>
+      </c>
+      <c r="P18">
+        <v>0.9</v>
+      </c>
+      <c r="Q18">
+        <v>7</v>
+      </c>
+      <c r="R18">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="1">
+        <v>79</v>
+      </c>
+      <c r="B19">
+        <v>79</v>
+      </c>
+      <c r="D19">
+        <v>35004095</v>
+      </c>
+      <c r="E19">
+        <v>85218177</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="O19">
+        <v>71.87</v>
+      </c>
+      <c r="P19">
+        <v>0.9</v>
+      </c>
+      <c r="Q19">
+        <v>7</v>
+      </c>
+      <c r="R19">
+        <v>7.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="1">
+        <v>82</v>
+      </c>
+      <c r="B20">
+        <v>82</v>
+      </c>
+      <c r="D20">
+        <v>35050668</v>
+      </c>
+      <c r="E20">
+        <v>85153075</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" t="s">
+        <v>53</v>
+      </c>
+      <c r="K20" t="s">
+        <v>57</v>
+      </c>
+      <c r="L20" t="s">
+        <v>60</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20">
+        <v>74.64</v>
+      </c>
+      <c r="O20">
+        <v>71.86</v>
+      </c>
+      <c r="P20">
+        <v>0.91</v>
+      </c>
+      <c r="Q20">
+        <v>7</v>
+      </c>
+      <c r="R20">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="1">
+        <v>82</v>
+      </c>
+      <c r="B21">
+        <v>82</v>
+      </c>
+      <c r="D21">
+        <v>35050668</v>
+      </c>
+      <c r="E21">
+        <v>85153075</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" t="s">
+        <v>53</v>
+      </c>
+      <c r="K21" t="s">
+        <v>57</v>
+      </c>
+      <c r="L21" t="s">
+        <v>60</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
+      <c r="N21">
+        <v>74.64</v>
+      </c>
+      <c r="O21">
+        <v>71.86</v>
+      </c>
+      <c r="P21">
+        <v>0.91</v>
+      </c>
+      <c r="Q21">
+        <v>7</v>
+      </c>
+      <c r="R21">
+        <v>6.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'Jere' of https://github.com/oitsjustjose/SCAL_USIgnite-911 into Jere"
This reverts commit 820b73cc87c199aab35efdb1122a06824e994c8f, reversing
changes made to f6fa092581434918fab24f62872697efe91a8870.
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/2018 Data/DailyReports/ToRemoveFile.xlsx
+++ b/Excel & CSV Sheets/2018 Data/DailyReports/ToRemoveFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="94">
   <si>
     <t>Index</t>
   </si>
@@ -112,43 +112,190 @@
     <t>ConditionBefore</t>
   </si>
   <si>
-    <t>2018-08-21</t>
-  </si>
-  <si>
-    <t>17:52:13</t>
-  </si>
-  <si>
-    <t>17:51:42</t>
-  </si>
-  <si>
-    <t>08:07:28</t>
-  </si>
-  <si>
-    <t>08:06:54</t>
+    <t>2018-08-16</t>
+  </si>
+  <si>
+    <t>23:08:56</t>
+  </si>
+  <si>
+    <t>18:16:11</t>
+  </si>
+  <si>
+    <t>18:14:35</t>
+  </si>
+  <si>
+    <t>17:35:05</t>
+  </si>
+  <si>
+    <t>17:20:57</t>
+  </si>
+  <si>
+    <t>17:04:39</t>
+  </si>
+  <si>
+    <t>16:28:29</t>
+  </si>
+  <si>
+    <t>16:17:23</t>
+  </si>
+  <si>
+    <t>15:54:31</t>
+  </si>
+  <si>
+    <t>15:41:14</t>
+  </si>
+  <si>
+    <t>15:31:02</t>
+  </si>
+  <si>
+    <t>14:47:01</t>
+  </si>
+  <si>
+    <t>12:57:03</t>
+  </si>
+  <si>
+    <t>12:57:02</t>
+  </si>
+  <si>
+    <t>12:10:43</t>
+  </si>
+  <si>
+    <t>12:10:24</t>
+  </si>
+  <si>
+    <t>11:41:06</t>
+  </si>
+  <si>
+    <t>11:36:07</t>
+  </si>
+  <si>
+    <t>11:36:00</t>
+  </si>
+  <si>
+    <t>11:24:42</t>
+  </si>
+  <si>
+    <t>11:20:13</t>
+  </si>
+  <si>
+    <t>08:07:21</t>
+  </si>
+  <si>
+    <t>00:28:45</t>
+  </si>
+  <si>
+    <t>Unknown Injuries</t>
   </si>
   <si>
     <t>Injuries</t>
   </si>
   <si>
-    <t>Brainerd Rd / N Germantown Rd</t>
-  </si>
-  <si>
-    <t>Brainerd Rd / Woodlawn Dr</t>
+    <t>No Injuries</t>
+  </si>
+  <si>
+    <t>18300 INTERSTATE 24 EB</t>
+  </si>
+  <si>
+    <t>2000 - 2099 Northpoint Blvd</t>
+  </si>
+  <si>
+    <t>18310 - 18399 Interstate 24 Eb</t>
+  </si>
+  <si>
+    <t>420 - 479 Interstate 75 Sb</t>
+  </si>
+  <si>
+    <t>Windsor St / Dodson Ave</t>
+  </si>
+  <si>
+    <t>18360 INTERSTATE 24 EB</t>
+  </si>
+  <si>
+    <t>18300 Interstate 24 Eb</t>
+  </si>
+  <si>
+    <t>3151 Broad St</t>
+  </si>
+  <si>
+    <t>Apison Pike / Little Debbie Pkwy</t>
+  </si>
+  <si>
+    <t>1 - 9 Exit Lee Hwy Off Ramp Sb</t>
+  </si>
+  <si>
+    <t>3550 W Rd</t>
+  </si>
+  <si>
+    <t>1200 Interstate 75 Nb</t>
+  </si>
+  <si>
+    <t>1009 W 39th St</t>
+  </si>
+  <si>
+    <t>COMMONS BLVD / GUNBARREL RD</t>
+  </si>
+  <si>
+    <t>Citico Ave / N Orchard Knob Ave</t>
+  </si>
+  <si>
+    <t>800 N ORCHARD KNOB AVE</t>
+  </si>
+  <si>
+    <t>Broad St / Cummings Hwy</t>
+  </si>
+  <si>
+    <t>Broad St / Old Wauhatchie Pike</t>
+  </si>
+  <si>
+    <t>7500 - 7539 E Brainerd Rd</t>
+  </si>
+  <si>
+    <t>205 Glenwood Dr</t>
+  </si>
+  <si>
+    <t>EAST RIDGE</t>
   </si>
   <si>
     <t>CHATTANOOGA</t>
   </si>
   <si>
+    <t>COLLEGEDALE</t>
+  </si>
+  <si>
+    <t>HAMILTON COUNTY</t>
+  </si>
+  <si>
+    <t>partly-cloudy-night</t>
+  </si>
+  <si>
     <t>partly-cloudy-day</t>
   </si>
   <si>
+    <t>clear-night</t>
+  </si>
+  <si>
     <t>Mostly Cloudy</t>
   </si>
   <si>
+    <t>Partly Cloudy</t>
+  </si>
+  <si>
+    <t>Humid and Partly Cloudy</t>
+  </si>
+  <si>
+    <t>Humid and Mostly Cloudy</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
     <t>rain</t>
   </si>
   <si>
-    <t>partly-cloudy-night</t>
+    <t>cloudy</t>
+  </si>
+  <si>
+    <t>Overcast</t>
   </si>
 </sst>
 </file>
@@ -506,7 +653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -612,16 +759,16 @@
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>35.024158</v>
+        <v>35.015818</v>
       </c>
       <c r="E2">
-        <v>-85.24646799999999</v>
+        <v>-85.254192</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
@@ -630,31 +777,31 @@
         <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="M2">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="N2">
-        <v>84.73</v>
+        <v>79.26000000000001</v>
       </c>
       <c r="O2">
-        <v>84.73</v>
+        <v>90.65000000000001</v>
       </c>
       <c r="P2">
-        <v>72.98</v>
+        <v>71.09999999999999</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -675,51 +822,48 @@
         <v>1</v>
       </c>
       <c r="W2">
-        <v>67.31999999999999</v>
+        <v>71.14</v>
       </c>
       <c r="X2">
-        <v>0.5600000000000001</v>
+        <v>0.76</v>
       </c>
       <c r="Y2">
         <v>8</v>
       </c>
       <c r="Z2">
-        <v>5.72</v>
+        <v>5.68</v>
       </c>
       <c r="AA2">
-        <v>0.83</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>43</v>
+        <v>0.43</v>
       </c>
       <c r="AC2">
-        <v>0.0008</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>0.0103</v>
+        <v>0.0003</v>
       </c>
       <c r="AE2">
-        <v>1534867200</v>
+        <v>1534464000</v>
       </c>
       <c r="AF2" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="AG2" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:33">
       <c r="A3" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>35.024158</v>
+        <v>35.13598</v>
       </c>
       <c r="E3">
-        <v>-85.24646799999999</v>
+        <v>-85.23961799999999</v>
       </c>
       <c r="F3" t="s">
         <v>32</v>
@@ -728,31 +872,31 @@
         <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="L3" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="M3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N3">
-        <v>84.73</v>
+        <v>87.34999999999999</v>
       </c>
       <c r="O3">
-        <v>84.73</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="P3">
-        <v>72.98</v>
+        <v>71.52</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -773,51 +917,51 @@
         <v>1</v>
       </c>
       <c r="W3">
-        <v>67.31999999999999</v>
+        <v>70.20999999999999</v>
       </c>
       <c r="X3">
-        <v>0.5600000000000001</v>
+        <v>0.57</v>
       </c>
       <c r="Y3">
         <v>8</v>
       </c>
       <c r="Z3">
-        <v>5.72</v>
+        <v>7.15</v>
       </c>
       <c r="AA3">
-        <v>0.83</v>
+        <v>0.44</v>
       </c>
       <c r="AB3" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="AC3">
-        <v>0.0008</v>
+        <v>0.0002</v>
       </c>
       <c r="AD3">
-        <v>0.0103</v>
+        <v>0.0016</v>
       </c>
       <c r="AE3">
-        <v>1534867200</v>
+        <v>1534464000</v>
       </c>
       <c r="AF3" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="AG3" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:33">
       <c r="A4" s="1">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>35.026267</v>
+        <v>35.13598</v>
       </c>
       <c r="E4">
-        <v>-85.25196099999999</v>
+        <v>-85.23961799999999</v>
       </c>
       <c r="F4" t="s">
         <v>32</v>
@@ -826,31 +970,31 @@
         <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="M4">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="N4">
-        <v>72.98999999999999</v>
+        <v>87.34999999999999</v>
       </c>
       <c r="O4">
-        <v>84.63</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="P4">
-        <v>72.88</v>
+        <v>71.52</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -871,51 +1015,51 @@
         <v>1</v>
       </c>
       <c r="W4">
-        <v>71.37</v>
+        <v>70.20999999999999</v>
       </c>
       <c r="X4">
-        <v>0.95</v>
+        <v>0.57</v>
       </c>
       <c r="Y4">
         <v>8</v>
       </c>
       <c r="Z4">
-        <v>5.54</v>
+        <v>7.15</v>
       </c>
       <c r="AA4">
-        <v>0.82</v>
+        <v>0.44</v>
       </c>
       <c r="AB4" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="AC4">
-        <v>0.0008</v>
+        <v>0.0002</v>
       </c>
       <c r="AD4">
-        <v>0.0103</v>
+        <v>0.0016</v>
       </c>
       <c r="AE4">
-        <v>1534867200</v>
+        <v>1534464000</v>
       </c>
       <c r="AF4" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="AG4" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:33">
       <c r="A5" s="1">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>35.026267</v>
+        <v>35.014338</v>
       </c>
       <c r="E5">
-        <v>-85.25196099999999</v>
+        <v>-85.25206900000001</v>
       </c>
       <c r="F5" t="s">
         <v>32</v>
@@ -924,31 +1068,31 @@
         <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="M5">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="N5">
-        <v>72.98999999999999</v>
+        <v>89.44</v>
       </c>
       <c r="O5">
-        <v>84.63</v>
+        <v>90.72</v>
       </c>
       <c r="P5">
-        <v>72.88</v>
+        <v>71.17</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -969,37 +1113,1851 @@
         <v>1</v>
       </c>
       <c r="W5">
-        <v>71.37</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="X5">
-        <v>0.95</v>
+        <v>0.51</v>
       </c>
       <c r="Y5">
         <v>8</v>
       </c>
       <c r="Z5">
-        <v>5.54</v>
+        <v>6.25</v>
       </c>
       <c r="AA5">
+        <v>0.43</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0.0003</v>
+      </c>
+      <c r="AE5">
+        <v>1534464000</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
+      <c r="A6" s="1">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>35.032543</v>
+      </c>
+      <c r="E6">
+        <v>-85.166732</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6">
+        <v>17</v>
+      </c>
+      <c r="N6">
+        <v>89.93000000000001</v>
+      </c>
+      <c r="O6">
+        <v>90.97</v>
+      </c>
+      <c r="P6">
+        <v>71.09</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>68.97</v>
+      </c>
+      <c r="X6">
+        <v>0.5</v>
+      </c>
+      <c r="Y6">
+        <v>8</v>
+      </c>
+      <c r="Z6">
+        <v>6.12</v>
+      </c>
+      <c r="AA6">
+        <v>0.39</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0.0002</v>
+      </c>
+      <c r="AE6">
+        <v>1534464000</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" s="1">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>35.047743</v>
+      </c>
+      <c r="E7">
+        <v>-85.26318999999999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7">
+        <v>17</v>
+      </c>
+      <c r="N7">
+        <v>89.62</v>
+      </c>
+      <c r="O7">
+        <v>90.98999999999999</v>
+      </c>
+      <c r="P7">
+        <v>71.47</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>68.91</v>
+      </c>
+      <c r="X7">
+        <v>0.51</v>
+      </c>
+      <c r="Y7">
+        <v>8</v>
+      </c>
+      <c r="Z7">
+        <v>6.24</v>
+      </c>
+      <c r="AA7">
+        <v>0.46</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0.0003</v>
+      </c>
+      <c r="AE7">
+        <v>1534464000</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" s="1">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>35.01101</v>
+      </c>
+      <c r="E8">
+        <v>-85.244051</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8">
+        <v>16</v>
+      </c>
+      <c r="N8">
+        <v>90.93000000000001</v>
+      </c>
+      <c r="O8">
+        <v>90.93000000000001</v>
+      </c>
+      <c r="P8">
+        <v>71.39</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>69.62</v>
+      </c>
+      <c r="X8">
+        <v>0.5</v>
+      </c>
+      <c r="Y8">
+        <v>8</v>
+      </c>
+      <c r="Z8">
+        <v>6.22</v>
+      </c>
+      <c r="AA8">
+        <v>0.42</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0.0003</v>
+      </c>
+      <c r="AE8">
+        <v>1534464000</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9" s="1">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>35.015818</v>
+      </c>
+      <c r="E9">
+        <v>-85.254192</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9">
+        <v>16</v>
+      </c>
+      <c r="N9">
+        <v>90.65000000000001</v>
+      </c>
+      <c r="O9">
+        <v>90.65000000000001</v>
+      </c>
+      <c r="P9">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>69.62</v>
+      </c>
+      <c r="X9">
+        <v>0.5</v>
+      </c>
+      <c r="Y9">
+        <v>8</v>
+      </c>
+      <c r="Z9">
+        <v>6.26</v>
+      </c>
+      <c r="AA9">
+        <v>0.43</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0.0003</v>
+      </c>
+      <c r="AE9">
+        <v>1534464000</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
+      <c r="A10" s="1">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>35.019269</v>
+      </c>
+      <c r="E10">
+        <v>-85.321684</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" t="s">
+        <v>86</v>
+      </c>
+      <c r="M10">
+        <v>15</v>
+      </c>
+      <c r="N10">
+        <v>90.47</v>
+      </c>
+      <c r="O10">
+        <v>91.22</v>
+      </c>
+      <c r="P10">
+        <v>71.70999999999999</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>69.92</v>
+      </c>
+      <c r="X10">
+        <v>0.51</v>
+      </c>
+      <c r="Y10">
+        <v>8</v>
+      </c>
+      <c r="Z10">
+        <v>2.75</v>
+      </c>
+      <c r="AA10">
+        <v>0.51</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC10">
+        <v>0.0001</v>
+      </c>
+      <c r="AD10">
+        <v>0.0008</v>
+      </c>
+      <c r="AE10">
+        <v>1534453200</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="A11" s="1">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <v>35.062983</v>
+      </c>
+      <c r="E11">
+        <v>-85.07423</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M11">
+        <v>15</v>
+      </c>
+      <c r="N11">
+        <v>89.79000000000001</v>
+      </c>
+      <c r="O11">
+        <v>90.73999999999999</v>
+      </c>
+      <c r="P11">
+        <v>70.81</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>70.34</v>
+      </c>
+      <c r="X11">
+        <v>0.53</v>
+      </c>
+      <c r="Y11">
+        <v>8</v>
+      </c>
+      <c r="Z11">
+        <v>6.37</v>
+      </c>
+      <c r="AA11">
+        <v>0.34</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0.0002</v>
+      </c>
+      <c r="AE11">
+        <v>1534464000</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="A12" s="1">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>51</v>
+      </c>
+      <c r="D12">
+        <v>35.036125</v>
+      </c>
+      <c r="E12">
+        <v>-85.18406</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K12" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" t="s">
+        <v>87</v>
+      </c>
+      <c r="M12">
+        <v>15</v>
+      </c>
+      <c r="N12">
+        <v>90.06</v>
+      </c>
+      <c r="O12">
+        <v>90.95999999999999</v>
+      </c>
+      <c r="P12">
+        <v>71.09</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>69.95</v>
+      </c>
+      <c r="X12">
+        <v>0.52</v>
+      </c>
+      <c r="Y12">
+        <v>8</v>
+      </c>
+      <c r="Z12">
+        <v>5.95</v>
+      </c>
+      <c r="AA12">
+        <v>0.4</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0.0002</v>
+      </c>
+      <c r="AE12">
+        <v>1534464000</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="A13" s="1">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>35.110565</v>
+      </c>
+      <c r="E13">
+        <v>-85.32789200000001</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" t="s">
+        <v>86</v>
+      </c>
+      <c r="M13">
+        <v>14</v>
+      </c>
+      <c r="N13">
+        <v>89.33</v>
+      </c>
+      <c r="O13">
+        <v>90.31</v>
+      </c>
+      <c r="P13">
+        <v>70.69</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>71.84</v>
+      </c>
+      <c r="X13">
+        <v>0.57</v>
+      </c>
+      <c r="Y13">
+        <v>8</v>
+      </c>
+      <c r="Z13">
+        <v>6.63</v>
+      </c>
+      <c r="AA13">
+        <v>0.47</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC13">
+        <v>0.0001</v>
+      </c>
+      <c r="AD13">
+        <v>0.0012</v>
+      </c>
+      <c r="AE13">
+        <v>1534453200</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
+      <c r="A14" s="1">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>62</v>
+      </c>
+      <c r="D14">
+        <v>35.090087</v>
+      </c>
+      <c r="E14">
+        <v>-85.06041</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <v>85.73999999999999</v>
+      </c>
+      <c r="O14">
+        <v>90.84999999999999</v>
+      </c>
+      <c r="P14">
+        <v>70.84</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>72.40000000000001</v>
+      </c>
+      <c r="X14">
+        <v>0.65</v>
+      </c>
+      <c r="Y14">
+        <v>8</v>
+      </c>
+      <c r="Z14">
+        <v>6.92</v>
+      </c>
+      <c r="AA14">
+        <v>0.33</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0.0002</v>
+      </c>
+      <c r="AE14">
+        <v>1534464000</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
+      <c r="A15" s="1">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>63</v>
+      </c>
+      <c r="D15">
+        <v>35.090087</v>
+      </c>
+      <c r="E15">
+        <v>-85.06041</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" t="s">
+        <v>84</v>
+      </c>
+      <c r="L15" t="s">
+        <v>88</v>
+      </c>
+      <c r="M15">
+        <v>12</v>
+      </c>
+      <c r="N15">
+        <v>85.73999999999999</v>
+      </c>
+      <c r="O15">
+        <v>90.84999999999999</v>
+      </c>
+      <c r="P15">
+        <v>70.84</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>72.40000000000001</v>
+      </c>
+      <c r="X15">
+        <v>0.65</v>
+      </c>
+      <c r="Y15">
+        <v>8</v>
+      </c>
+      <c r="Z15">
+        <v>6.92</v>
+      </c>
+      <c r="AA15">
+        <v>0.33</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0.0002</v>
+      </c>
+      <c r="AE15">
+        <v>1534464000</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33">
+      <c r="A16" s="1">
+        <v>74</v>
+      </c>
+      <c r="B16">
+        <v>74</v>
+      </c>
+      <c r="D16">
+        <v>35.008587</v>
+      </c>
+      <c r="E16">
+        <v>-85.321031</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" t="s">
+        <v>89</v>
+      </c>
+      <c r="M16">
+        <v>12</v>
+      </c>
+      <c r="N16">
+        <v>85.95999999999999</v>
+      </c>
+      <c r="O16">
+        <v>91.16</v>
+      </c>
+      <c r="P16">
+        <v>71.68000000000001</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>72.56999999999999</v>
+      </c>
+      <c r="X16">
+        <v>0.65</v>
+      </c>
+      <c r="Y16">
+        <v>8</v>
+      </c>
+      <c r="Z16">
+        <v>2.28</v>
+      </c>
+      <c r="AA16">
+        <v>0.51</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0.0003</v>
+      </c>
+      <c r="AE16">
+        <v>1534464000</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33">
+      <c r="A17" s="1">
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <v>75</v>
+      </c>
+      <c r="D17">
+        <v>35.008587</v>
+      </c>
+      <c r="E17">
+        <v>-85.321031</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" t="s">
+        <v>80</v>
+      </c>
+      <c r="K17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17">
+        <v>12</v>
+      </c>
+      <c r="N17">
+        <v>85.95999999999999</v>
+      </c>
+      <c r="O17">
+        <v>91.16</v>
+      </c>
+      <c r="P17">
+        <v>71.68000000000001</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>72.56999999999999</v>
+      </c>
+      <c r="X17">
+        <v>0.65</v>
+      </c>
+      <c r="Y17">
+        <v>8</v>
+      </c>
+      <c r="Z17">
+        <v>2.28</v>
+      </c>
+      <c r="AA17">
+        <v>0.51</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0.0003</v>
+      </c>
+      <c r="AE17">
+        <v>1534464000</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33">
+      <c r="A18" s="1">
+        <v>84</v>
+      </c>
+      <c r="B18">
+        <v>84</v>
+      </c>
+      <c r="D18">
+        <v>35.036959</v>
+      </c>
+      <c r="E18">
+        <v>-85.15182299999999</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" t="s">
+        <v>87</v>
+      </c>
+      <c r="M18">
+        <v>11</v>
+      </c>
+      <c r="N18">
+        <v>83.34</v>
+      </c>
+      <c r="O18">
+        <v>90.98999999999999</v>
+      </c>
+      <c r="P18">
+        <v>71.11</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>71.89</v>
+      </c>
+      <c r="X18">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="Y18">
+        <v>8</v>
+      </c>
+      <c r="Z18">
+        <v>5.91</v>
+      </c>
+      <c r="AA18">
+        <v>0.38</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0.0002</v>
+      </c>
+      <c r="AE18">
+        <v>1534464000</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33">
+      <c r="A19" s="1">
+        <v>86</v>
+      </c>
+      <c r="B19">
+        <v>86</v>
+      </c>
+      <c r="D19">
+        <v>35.045878</v>
+      </c>
+      <c r="E19">
+        <v>-85.269401</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" t="s">
+        <v>73</v>
+      </c>
+      <c r="J19" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" t="s">
+        <v>86</v>
+      </c>
+      <c r="M19">
+        <v>11</v>
+      </c>
+      <c r="N19">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="O19">
+        <v>91.18000000000001</v>
+      </c>
+      <c r="P19">
+        <v>71.66</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>71.90000000000001</v>
+      </c>
+      <c r="X19">
+        <v>0.68</v>
+      </c>
+      <c r="Y19">
+        <v>8</v>
+      </c>
+      <c r="Z19">
+        <v>6.25</v>
+      </c>
+      <c r="AA19">
+        <v>0.47</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0.0003</v>
+      </c>
+      <c r="AE19">
+        <v>1534464000</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33">
+      <c r="A20" s="1">
+        <v>87</v>
+      </c>
+      <c r="B20">
+        <v>87</v>
+      </c>
+      <c r="D20">
+        <v>35.045878</v>
+      </c>
+      <c r="E20">
+        <v>-85.269401</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" t="s">
+        <v>80</v>
+      </c>
+      <c r="K20" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" t="s">
+        <v>86</v>
+      </c>
+      <c r="M20">
+        <v>11</v>
+      </c>
+      <c r="N20">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="O20">
+        <v>91.18000000000001</v>
+      </c>
+      <c r="P20">
+        <v>71.66</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>71.90000000000001</v>
+      </c>
+      <c r="X20">
+        <v>0.68</v>
+      </c>
+      <c r="Y20">
+        <v>8</v>
+      </c>
+      <c r="Z20">
+        <v>6.25</v>
+      </c>
+      <c r="AA20">
+        <v>0.47</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0.0003</v>
+      </c>
+      <c r="AE20">
+        <v>1534464000</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33">
+      <c r="A21" s="1">
+        <v>89</v>
+      </c>
+      <c r="B21">
+        <v>89</v>
+      </c>
+      <c r="D21">
+        <v>35.013727</v>
+      </c>
+      <c r="E21">
+        <v>-85.32828499999999</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" t="s">
+        <v>80</v>
+      </c>
+      <c r="K21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" t="s">
+        <v>86</v>
+      </c>
+      <c r="M21">
+        <v>11</v>
+      </c>
+      <c r="N21">
+        <v>83.2</v>
+      </c>
+      <c r="O21">
+        <v>91.09</v>
+      </c>
+      <c r="P21">
+        <v>71.58</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>71.83</v>
+      </c>
+      <c r="X21">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="Y21">
+        <v>8</v>
+      </c>
+      <c r="Z21">
+        <v>3.42</v>
+      </c>
+      <c r="AA21">
+        <v>0.51</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC21">
+        <v>0.0001</v>
+      </c>
+      <c r="AD21">
+        <v>0.0008</v>
+      </c>
+      <c r="AE21">
+        <v>1534453200</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33">
+      <c r="A22" s="1">
+        <v>90</v>
+      </c>
+      <c r="B22">
+        <v>90</v>
+      </c>
+      <c r="D22">
+        <v>35.013727</v>
+      </c>
+      <c r="E22">
+        <v>-85.32828499999999</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J22" t="s">
+        <v>80</v>
+      </c>
+      <c r="K22" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" t="s">
+        <v>86</v>
+      </c>
+      <c r="M22">
+        <v>11</v>
+      </c>
+      <c r="N22">
+        <v>83.2</v>
+      </c>
+      <c r="O22">
+        <v>91.09</v>
+      </c>
+      <c r="P22">
+        <v>71.58</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>71.83</v>
+      </c>
+      <c r="X22">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="Y22">
+        <v>8</v>
+      </c>
+      <c r="Z22">
+        <v>3.42</v>
+      </c>
+      <c r="AA22">
+        <v>0.51</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC22">
+        <v>0.0001</v>
+      </c>
+      <c r="AD22">
+        <v>0.0008</v>
+      </c>
+      <c r="AE22">
+        <v>1534453200</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33">
+      <c r="A23" s="1">
+        <v>105</v>
+      </c>
+      <c r="B23">
+        <v>105</v>
+      </c>
+      <c r="D23">
+        <v>35.013797</v>
+      </c>
+      <c r="E23">
+        <v>-85.16132</v>
+      </c>
+      <c r="F23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" t="s">
+        <v>80</v>
+      </c>
+      <c r="K23" t="s">
+        <v>84</v>
+      </c>
+      <c r="L23" t="s">
+        <v>87</v>
+      </c>
+      <c r="M23">
+        <v>8</v>
+      </c>
+      <c r="N23">
+        <v>72.09</v>
+      </c>
+      <c r="O23">
+        <v>91.06999999999999</v>
+      </c>
+      <c r="P23">
+        <v>71.2</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>67.88</v>
+      </c>
+      <c r="X23">
+        <v>0.87</v>
+      </c>
+      <c r="Y23">
+        <v>8</v>
+      </c>
+      <c r="Z23">
+        <v>3.78</v>
+      </c>
+      <c r="AA23">
+        <v>0.39</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0.0002</v>
+      </c>
+      <c r="AE23">
+        <v>1534464000</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33">
+      <c r="A24" s="1">
+        <v>111</v>
+      </c>
+      <c r="B24">
+        <v>111</v>
+      </c>
+      <c r="D24">
+        <v>35.033982</v>
+      </c>
+      <c r="E24">
+        <v>-85.263012</v>
+      </c>
+      <c r="F24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" t="s">
+        <v>78</v>
+      </c>
+      <c r="J24" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24" t="s">
+        <v>85</v>
+      </c>
+      <c r="L24" t="s">
+        <v>90</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>71.95999999999999</v>
+      </c>
+      <c r="O24">
+        <v>89.04000000000001</v>
+      </c>
+      <c r="P24">
+        <v>67.83</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>66.15000000000001</v>
+      </c>
+      <c r="X24">
         <v>0.82</v>
       </c>
-      <c r="AB5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC5">
-        <v>0.0008</v>
-      </c>
-      <c r="AD5">
-        <v>0.0103</v>
-      </c>
-      <c r="AE5">
-        <v>1534867200</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>42</v>
+      <c r="Y24">
+        <v>8</v>
+      </c>
+      <c r="Z24">
+        <v>5.85</v>
+      </c>
+      <c r="AA24">
+        <v>0.49</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0.0003</v>
+      </c>
+      <c r="AE24">
+        <v>1534374000</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned alot of folders
</commit_message>
<xml_diff>
--- a/Excel & CSV Sheets/2018 Data/DailyReports/ToRemoveFile.xlsx
+++ b/Excel & CSV Sheets/2018 Data/DailyReports/ToRemoveFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="100">
   <si>
     <t>Accident</t>
   </si>
@@ -175,181 +175,127 @@
     <t>Injuries</t>
   </si>
   <si>
+    <t>Entrapment</t>
+  </si>
+  <si>
     <t>Unknown Injuries</t>
   </si>
   <si>
-    <t>Entrapment</t>
-  </si>
-  <si>
-    <t>2018-11-06</t>
-  </si>
-  <si>
-    <t>22:35:04</t>
-  </si>
-  <si>
-    <t>22:34:28</t>
-  </si>
-  <si>
-    <t>18:12:33</t>
-  </si>
-  <si>
-    <t>18:11:59</t>
-  </si>
-  <si>
-    <t>16:06:51</t>
-  </si>
-  <si>
-    <t>16:06:21</t>
-  </si>
-  <si>
-    <t>15:51:11</t>
-  </si>
-  <si>
-    <t>15:34:13</t>
-  </si>
-  <si>
-    <t>14:06:49</t>
-  </si>
-  <si>
-    <t>13:13:59</t>
-  </si>
-  <si>
-    <t>13:12:32</t>
-  </si>
-  <si>
-    <t>11:36:06</t>
-  </si>
-  <si>
-    <t>11:08:29</t>
-  </si>
-  <si>
-    <t>11:07:52</t>
-  </si>
-  <si>
-    <t>10:47:05</t>
-  </si>
-  <si>
-    <t>10:46:43</t>
-  </si>
-  <si>
-    <t>10:46:34</t>
-  </si>
-  <si>
-    <t>10:36:51</t>
-  </si>
-  <si>
-    <t>10:32:22</t>
-  </si>
-  <si>
-    <t>10:31:46</t>
-  </si>
-  <si>
-    <t>08:55:52</t>
-  </si>
-  <si>
-    <t>08:35:03</t>
-  </si>
-  <si>
-    <t>08:04:36</t>
-  </si>
-  <si>
-    <t>07:24:25</t>
-  </si>
-  <si>
-    <t>07:18:11</t>
-  </si>
-  <si>
-    <t>07:17:02</t>
-  </si>
-  <si>
-    <t>06:27:57</t>
-  </si>
-  <si>
-    <t>03:00:34</t>
-  </si>
-  <si>
-    <t>1809 Dodson Ave</t>
-  </si>
-  <si>
-    <t>4700 Wesleyan Rd</t>
-  </si>
-  <si>
-    <t>1440 Interstate 75 Sb</t>
-  </si>
-  <si>
-    <t>1330 - 1560 Interstate 75 Sb</t>
-  </si>
-  <si>
-    <t>Woodland Dr / Bill Reed Rd</t>
-  </si>
-  <si>
-    <t>Shallowford Rd / N Moore Rd</t>
-  </si>
-  <si>
-    <t>2215 VANCE AVE</t>
-  </si>
-  <si>
-    <t>2128 Citico Ave</t>
-  </si>
-  <si>
-    <t>Friar Rd / Central Dr</t>
-  </si>
-  <si>
-    <t>300 CENTRAL DR</t>
-  </si>
-  <si>
-    <t>5579 Highway 153</t>
-  </si>
-  <si>
-    <t>5579 HIGHWAY 153</t>
-  </si>
-  <si>
-    <t>1318 S Seminole Dr</t>
-  </si>
-  <si>
-    <t>4131 Ringgold Rd</t>
-  </si>
-  <si>
-    <t>4106 W RD</t>
-  </si>
-  <si>
-    <t>7499 BONNY OAKS DR</t>
-  </si>
-  <si>
-    <t>17180 Interstate 24 Eb</t>
-  </si>
-  <si>
-    <t>420 O Neal St</t>
-  </si>
-  <si>
-    <t>1030 Oak St</t>
-  </si>
-  <si>
-    <t>9414 Dallas Hollow Rd</t>
-  </si>
-  <si>
-    <t>641 HIGHWAY 27 NB</t>
+    <t>2018-11-12</t>
+  </si>
+  <si>
+    <t>23:19:05</t>
+  </si>
+  <si>
+    <t>23:18:18</t>
+  </si>
+  <si>
+    <t>17:53:23</t>
+  </si>
+  <si>
+    <t>17:23:13</t>
+  </si>
+  <si>
+    <t>17:21:48</t>
+  </si>
+  <si>
+    <t>17:16:58</t>
+  </si>
+  <si>
+    <t>17:14:48</t>
+  </si>
+  <si>
+    <t>17:03:02</t>
+  </si>
+  <si>
+    <t>15:42:31</t>
+  </si>
+  <si>
+    <t>14:28:23</t>
+  </si>
+  <si>
+    <t>12:02:16</t>
+  </si>
+  <si>
+    <t>12:00:28</t>
+  </si>
+  <si>
+    <t>10:00:38</t>
+  </si>
+  <si>
+    <t>09:54:06</t>
+  </si>
+  <si>
+    <t>09:52:22</t>
+  </si>
+  <si>
+    <t>09:49:36</t>
+  </si>
+  <si>
+    <t>09:05:38</t>
+  </si>
+  <si>
+    <t>08:59:12</t>
+  </si>
+  <si>
+    <t>08:58:03</t>
+  </si>
+  <si>
+    <t>18100 Interstate 24 Eb</t>
+  </si>
+  <si>
+    <t>420 - 479 Interstate 75 Sb</t>
+  </si>
+  <si>
+    <t>3000-3099 Dodds Ave</t>
+  </si>
+  <si>
+    <t>100 Interstate 75 Sb</t>
+  </si>
+  <si>
+    <t>Glass St / Campbell St</t>
+  </si>
+  <si>
+    <t>E 11th St / Peeples St</t>
+  </si>
+  <si>
+    <t>18260 INTERSTATE 24 WB</t>
+  </si>
+  <si>
+    <t>1157 Mountain Creek Rd</t>
+  </si>
+  <si>
+    <t>301-319 E Martin Luther King Blvd</t>
+  </si>
+  <si>
+    <t>801-899 Houston St</t>
+  </si>
+  <si>
+    <t>11600-12106 HIGHWAY 111 SB</t>
+  </si>
+  <si>
+    <t>12108-13098 Highway 111 Nb</t>
+  </si>
+  <si>
+    <t>12108-13099 HIGHWAY 111 NB</t>
   </si>
   <si>
     <t>CHATTANOOGA</t>
   </si>
   <si>
+    <t>EAST RIDGE</t>
+  </si>
+  <si>
+    <t>SODDY DAISY</t>
+  </si>
+  <si>
     <t>HAMILTON COUNTY</t>
   </si>
   <si>
-    <t>EAST RIDGE</t>
-  </si>
-  <si>
-    <t>RED BANK</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>16</t>
+    <t>23</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
   <si>
     <t>15</t>
@@ -358,25 +304,16 @@
     <t>14</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>11</t>
+    <t>12</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>8</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
 </sst>
 </file>
@@ -734,7 +671,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA31"/>
+  <dimension ref="A1:BA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -900,16 +837,16 @@
     </row>
     <row r="2" spans="1:53">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>
       </c>
       <c r="D2">
-        <v>35.057199</v>
+        <v>35.016491</v>
       </c>
       <c r="E2">
-        <v>-85.258551</v>
+        <v>-85.28069000000001</v>
       </c>
       <c r="F2" t="s">
         <v>55</v>
@@ -918,13 +855,13 @@
         <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="K2" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="P2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="Y2">
         <v>11</v>
@@ -932,16 +869,16 @@
     </row>
     <row r="3" spans="1:53">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
       </c>
       <c r="D3">
-        <v>35.057199</v>
+        <v>35.016491</v>
       </c>
       <c r="E3">
-        <v>-85.258551</v>
+        <v>-85.28069000000001</v>
       </c>
       <c r="F3" t="s">
         <v>55</v>
@@ -950,13 +887,13 @@
         <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="K3" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="P3" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="Y3">
         <v>11</v>
@@ -964,16 +901,16 @@
     </row>
     <row r="4" spans="1:53">
       <c r="A4" s="1">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
       </c>
       <c r="D4">
-        <v>35.005983</v>
+        <v>35.027345</v>
       </c>
       <c r="E4">
-        <v>-84.97447699999999</v>
+        <v>-85.17252999999999</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
@@ -982,13 +919,13 @@
         <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K4" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="P4" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="Y4">
         <v>11</v>
@@ -996,16 +933,16 @@
     </row>
     <row r="5" spans="1:53">
       <c r="A5" s="1">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5">
-        <v>35.005983</v>
+        <v>35.006002</v>
       </c>
       <c r="E5">
-        <v>-84.97447699999999</v>
+        <v>-85.278818</v>
       </c>
       <c r="F5" t="s">
         <v>55</v>
@@ -1014,13 +951,13 @@
         <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="K5" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="P5" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="Y5">
         <v>11</v>
@@ -1028,16 +965,16 @@
     </row>
     <row r="6" spans="1:53">
       <c r="A6" s="1">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>52</v>
       </c>
       <c r="D6">
-        <v>35.12014</v>
+        <v>35.006002</v>
       </c>
       <c r="E6">
-        <v>-85.044089</v>
+        <v>-85.278818</v>
       </c>
       <c r="F6" t="s">
         <v>55</v>
@@ -1046,13 +983,13 @@
         <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="P6" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="Y6">
         <v>11</v>
@@ -1060,16 +997,16 @@
     </row>
     <row r="7" spans="1:53">
       <c r="A7" s="1">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>52</v>
       </c>
       <c r="D7">
-        <v>35.12014</v>
+        <v>34.998664</v>
       </c>
       <c r="E7">
-        <v>-85.044089</v>
+        <v>-85.20989400000001</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
@@ -1078,13 +1015,13 @@
         <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="K7" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="P7" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="Y7">
         <v>11</v>
@@ -1092,16 +1029,16 @@
     </row>
     <row r="8" spans="1:53">
       <c r="A8" s="1">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
         <v>52</v>
       </c>
       <c r="D8">
-        <v>35.105449</v>
+        <v>34.998664</v>
       </c>
       <c r="E8">
-        <v>-85.051768</v>
+        <v>-85.20989400000001</v>
       </c>
       <c r="F8" t="s">
         <v>55</v>
@@ -1110,13 +1047,13 @@
         <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="K8" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="P8" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="Y8">
         <v>11</v>
@@ -1124,16 +1061,16 @@
     </row>
     <row r="9" spans="1:53">
       <c r="A9" s="1">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9">
-        <v>35.04496</v>
+        <v>34.998664</v>
       </c>
       <c r="E9">
-        <v>-85.09841</v>
+        <v>-85.20989400000001</v>
       </c>
       <c r="F9" t="s">
         <v>55</v>
@@ -1142,13 +1079,13 @@
         <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="K9" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="P9" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="Y9">
         <v>11</v>
@@ -1156,16 +1093,16 @@
     </row>
     <row r="10" spans="1:53">
       <c r="A10" s="1">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
       </c>
       <c r="D10">
-        <v>35.043284</v>
+        <v>35.067236</v>
       </c>
       <c r="E10">
-        <v>-85.219735</v>
+        <v>-85.243306</v>
       </c>
       <c r="F10" t="s">
         <v>55</v>
@@ -1174,13 +1111,13 @@
         <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="K10" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="P10" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="Y10">
         <v>11</v>
@@ -1188,16 +1125,16 @@
     </row>
     <row r="11" spans="1:53">
       <c r="A11" s="1">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
       </c>
       <c r="D11">
-        <v>35.029051</v>
+        <v>35.040031</v>
       </c>
       <c r="E11">
-        <v>-85.27175699999999</v>
+        <v>-85.299344</v>
       </c>
       <c r="F11" t="s">
         <v>55</v>
@@ -1206,13 +1143,13 @@
         <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="K11" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="P11" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Y11">
         <v>11</v>
@@ -1220,16 +1157,16 @@
     </row>
     <row r="12" spans="1:53">
       <c r="A12" s="1">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="C12" t="s">
         <v>52</v>
       </c>
       <c r="D12">
-        <v>35.029051</v>
+        <v>35.019555</v>
       </c>
       <c r="E12">
-        <v>-85.27175699999999</v>
+        <v>-85.258653</v>
       </c>
       <c r="F12" t="s">
         <v>55</v>
@@ -1238,13 +1175,13 @@
         <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="K12" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="P12" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="Y12">
         <v>11</v>
@@ -1252,16 +1189,16 @@
     </row>
     <row r="13" spans="1:53">
       <c r="A13" s="1">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
         <v>52</v>
       </c>
       <c r="D13">
-        <v>35.043886</v>
+        <v>35.019555</v>
       </c>
       <c r="E13">
-        <v>-85.264904</v>
+        <v>-85.258653</v>
       </c>
       <c r="F13" t="s">
         <v>55</v>
@@ -1270,13 +1207,13 @@
         <v>67</v>
       </c>
       <c r="H13" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="K13" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="P13" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="Y13">
         <v>11</v>
@@ -1284,16 +1221,16 @@
     </row>
     <row r="14" spans="1:53">
       <c r="A14" s="1">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
       </c>
       <c r="D14">
-        <v>35.019236</v>
+        <v>35.116996</v>
       </c>
       <c r="E14">
-        <v>-85.197239</v>
+        <v>-85.318253</v>
       </c>
       <c r="F14" t="s">
         <v>55</v>
@@ -1302,13 +1239,13 @@
         <v>68</v>
       </c>
       <c r="H14" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="K14" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="P14" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="Y14">
         <v>11</v>
@@ -1316,16 +1253,16 @@
     </row>
     <row r="15" spans="1:53">
       <c r="A15" s="1">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
         <v>52</v>
       </c>
       <c r="D15">
-        <v>35.019236</v>
+        <v>35.04473</v>
       </c>
       <c r="E15">
-        <v>-85.197239</v>
+        <v>-85.30549000000001</v>
       </c>
       <c r="F15" t="s">
         <v>55</v>
@@ -1334,13 +1271,13 @@
         <v>69</v>
       </c>
       <c r="H15" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="K15" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="P15" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="Y15">
         <v>11</v>
@@ -1348,16 +1285,16 @@
     </row>
     <row r="16" spans="1:53">
       <c r="A16" s="1">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
       </c>
       <c r="D16">
-        <v>35.146073</v>
+        <v>35.04473</v>
       </c>
       <c r="E16">
-        <v>-85.25221500000001</v>
+        <v>-85.30549000000001</v>
       </c>
       <c r="F16" t="s">
         <v>55</v>
@@ -1366,13 +1303,13 @@
         <v>70</v>
       </c>
       <c r="H16" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="K16" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="P16" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="Y16">
         <v>11</v>
@@ -1380,16 +1317,16 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="1">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17">
-        <v>35.146073</v>
+        <v>35.0448</v>
       </c>
       <c r="E17">
-        <v>-85.25221500000001</v>
+        <v>-85.30556</v>
       </c>
       <c r="F17" t="s">
         <v>55</v>
@@ -1398,13 +1335,13 @@
         <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K17" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="P17" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="Y17">
         <v>11</v>
@@ -1412,31 +1349,31 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="1">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18">
-        <v>35.146073</v>
+        <v>35.0448</v>
       </c>
       <c r="E18">
-        <v>-85.25221500000001</v>
+        <v>-85.30556</v>
       </c>
       <c r="F18" t="s">
         <v>55</v>
       </c>
       <c r="G18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="K18" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="P18" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="Y18">
         <v>11</v>
@@ -1444,16 +1381,16 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="1">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19">
-        <v>35.146073</v>
+        <v>35.30606</v>
       </c>
       <c r="E19">
-        <v>-85.25221500000001</v>
+        <v>-85.16413</v>
       </c>
       <c r="F19" t="s">
         <v>55</v>
@@ -1462,13 +1399,13 @@
         <v>72</v>
       </c>
       <c r="H19" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="K19" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="P19" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="Y19">
         <v>11</v>
@@ -1476,16 +1413,16 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="1">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D20">
-        <v>34.994955</v>
+        <v>35.31551</v>
       </c>
       <c r="E20">
-        <v>-85.268467</v>
+        <v>-85.16149</v>
       </c>
       <c r="F20" t="s">
         <v>55</v>
@@ -1494,13 +1431,13 @@
         <v>73</v>
       </c>
       <c r="H20" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="K20" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="P20" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="Y20">
         <v>11</v>
@@ -1508,16 +1445,16 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="1">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D21">
-        <v>34.997998</v>
+        <v>35.311505</v>
       </c>
       <c r="E21">
-        <v>-85.245493</v>
+        <v>-85.16298</v>
       </c>
       <c r="F21" t="s">
         <v>55</v>
@@ -1526,335 +1463,15 @@
         <v>74</v>
       </c>
       <c r="H21" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="K21" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="P21" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="Y21">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25">
-      <c r="A22" s="1">
-        <v>98</v>
-      </c>
-      <c r="C22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22">
-        <v>34.997998</v>
-      </c>
-      <c r="E22">
-        <v>-85.245493</v>
-      </c>
-      <c r="F22" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" t="s">
-        <v>75</v>
-      </c>
-      <c r="H22" t="s">
-        <v>97</v>
-      </c>
-      <c r="K22" t="s">
-        <v>107</v>
-      </c>
-      <c r="P22" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y22">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25">
-      <c r="A23" s="1">
-        <v>109</v>
-      </c>
-      <c r="C23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23">
-        <v>35.129749</v>
-      </c>
-      <c r="E23">
-        <v>-85.317736</v>
-      </c>
-      <c r="F23" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" t="s">
-        <v>76</v>
-      </c>
-      <c r="H23" t="s">
-        <v>98</v>
-      </c>
-      <c r="K23" t="s">
-        <v>106</v>
-      </c>
-      <c r="P23" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y23">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
-      <c r="A24" s="1">
-        <v>112</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24">
-        <v>35.060689</v>
-      </c>
-      <c r="E24">
-        <v>-85.13423899999999</v>
-      </c>
-      <c r="F24" t="s">
-        <v>55</v>
-      </c>
-      <c r="G24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H24" t="s">
-        <v>99</v>
-      </c>
-      <c r="K24" t="s">
-        <v>105</v>
-      </c>
-      <c r="P24" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y24">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25">
-      <c r="A25" s="1">
-        <v>119</v>
-      </c>
-      <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25">
-        <v>34.9933</v>
-      </c>
-      <c r="E25">
-        <v>-85.399306</v>
-      </c>
-      <c r="F25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G25" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" t="s">
-        <v>100</v>
-      </c>
-      <c r="K25" t="s">
-        <v>105</v>
-      </c>
-      <c r="P25" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y25">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25">
-      <c r="A26" s="1">
-        <v>120</v>
-      </c>
-      <c r="C26" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26">
-        <v>34.9933</v>
-      </c>
-      <c r="E26">
-        <v>-85.399306</v>
-      </c>
-      <c r="F26" t="s">
-        <v>55</v>
-      </c>
-      <c r="G26" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26" t="s">
-        <v>100</v>
-      </c>
-      <c r="K26" t="s">
-        <v>105</v>
-      </c>
-      <c r="P26" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y26">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25">
-      <c r="A27" s="1">
-        <v>128</v>
-      </c>
-      <c r="C27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27">
-        <v>35.045143</v>
-      </c>
-      <c r="E27">
-        <v>-85.287233</v>
-      </c>
-      <c r="F27" t="s">
-        <v>55</v>
-      </c>
-      <c r="G27" t="s">
-        <v>79</v>
-      </c>
-      <c r="H27" t="s">
-        <v>101</v>
-      </c>
-      <c r="K27" t="s">
-        <v>105</v>
-      </c>
-      <c r="P27" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y27">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
-      <c r="A28" s="1">
-        <v>131</v>
-      </c>
-      <c r="C28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28">
-        <v>35.042179</v>
-      </c>
-      <c r="E28">
-        <v>-85.28935</v>
-      </c>
-      <c r="F28" t="s">
-        <v>55</v>
-      </c>
-      <c r="G28" t="s">
-        <v>80</v>
-      </c>
-      <c r="H28" t="s">
-        <v>102</v>
-      </c>
-      <c r="K28" t="s">
-        <v>105</v>
-      </c>
-      <c r="P28" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y28">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
-      <c r="A29" s="1">
-        <v>132</v>
-      </c>
-      <c r="C29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29">
-        <v>35.042179</v>
-      </c>
-      <c r="E29">
-        <v>-85.28935</v>
-      </c>
-      <c r="F29" t="s">
-        <v>55</v>
-      </c>
-      <c r="G29" t="s">
-        <v>81</v>
-      </c>
-      <c r="H29" t="s">
-        <v>102</v>
-      </c>
-      <c r="K29" t="s">
-        <v>105</v>
-      </c>
-      <c r="P29" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y29">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25">
-      <c r="A30" s="1">
-        <v>136</v>
-      </c>
-      <c r="C30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30">
-        <v>35.229566</v>
-      </c>
-      <c r="E30">
-        <v>-85.151321</v>
-      </c>
-      <c r="F30" t="s">
-        <v>55</v>
-      </c>
-      <c r="G30" t="s">
-        <v>82</v>
-      </c>
-      <c r="H30" t="s">
-        <v>103</v>
-      </c>
-      <c r="K30" t="s">
-        <v>106</v>
-      </c>
-      <c r="P30" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y30">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25">
-      <c r="A31" s="1">
-        <v>140</v>
-      </c>
-      <c r="C31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31">
-        <v>35.11613</v>
-      </c>
-      <c r="E31">
-        <v>-85.30224800000001</v>
-      </c>
-      <c r="F31" t="s">
-        <v>55</v>
-      </c>
-      <c r="G31" t="s">
-        <v>83</v>
-      </c>
-      <c r="H31" t="s">
-        <v>104</v>
-      </c>
-      <c r="K31" t="s">
-        <v>108</v>
-      </c>
-      <c r="P31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y31">
         <v>11</v>
       </c>
     </row>

</xml_diff>